<commit_message>
PCB: last BOM update before ordering
</commit_message>
<xml_diff>
--- a/2401-pcb/2401-pcb.xlsx
+++ b/2401-pcb/2401-pcb.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="162">
   <si>
     <t xml:space="preserve">Sync</t>
   </si>
@@ -260,6 +260,9 @@
   </si>
   <si>
     <t xml:space="preserve">2981749</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 versies van deze phototransistor: evt vergelijken</t>
   </si>
   <si>
     <t xml:space="preserve">Q2,</t>
@@ -546,12 +549,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDFCCE4"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -588,7 +597,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,6 +618,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -618,6 +631,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDFCCE4"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -628,8 +701,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,7 +783,7 @@
       <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1" t="n">
+      <c r="J2" s="5" t="n">
         <f aca="false">MAX(0,L$1*C2-K2)</f>
         <v>3</v>
       </c>
@@ -740,7 +813,7 @@
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="1" t="n">
+      <c r="J3" s="5" t="n">
         <f aca="false">MAX(0,L$1*C3-K3)</f>
         <v>3</v>
       </c>
@@ -767,7 +840,7 @@
       <c r="H4" s="2" t="n">
         <v>721980</v>
       </c>
-      <c r="J4" s="1" t="n">
+      <c r="J4" s="5" t="n">
         <f aca="false">MAX(0,L$1*C4-K4)</f>
         <v>6</v>
       </c>
@@ -794,7 +867,7 @@
       <c r="H5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="J5" s="5" t="n">
         <f aca="false">MAX(0,L$1*C5-K5)</f>
         <v>15</v>
       </c>
@@ -821,7 +894,7 @@
       <c r="H6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="J6" s="5" t="n">
         <f aca="false">MAX(0,L$1*C6-K6)</f>
         <v>48</v>
       </c>
@@ -851,7 +924,7 @@
       <c r="H7" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="J7" s="5" t="n">
         <f aca="false">MAX(0,L$1*C7-K7)</f>
         <v>3</v>
       </c>
@@ -881,7 +954,7 @@
       <c r="H8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="J8" s="5" t="n">
         <f aca="false">MAX(0,L$1*C8-K8)</f>
         <v>3</v>
       </c>
@@ -911,7 +984,7 @@
       <c r="H9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="J9" s="5" t="n">
         <f aca="false">MAX(0,L$1*C9-K9)</f>
         <v>3</v>
       </c>
@@ -941,7 +1014,7 @@
       <c r="H10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J10" s="1" t="n">
+      <c r="J10" s="5" t="n">
         <f aca="false">MAX(0,L$1*C10-K10)</f>
         <v>3</v>
       </c>
@@ -1055,15 +1128,18 @@
       <c r="F14" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="4" t="s">
         <v>78</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="J14" s="5" t="n">
         <f aca="false">MAX(0,L$1*C14-K14)</f>
         <v>3</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1071,13 +1147,13 @@
         <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>76</v>
@@ -1085,13 +1161,13 @@
       <c r="F15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>81</v>
+      <c r="G15" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="J15" s="5" t="n">
         <f aca="false">MAX(0,L$1*C15-K15)</f>
         <v>3</v>
       </c>
@@ -1101,24 +1177,24 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="J16" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="J16" s="5" t="n">
         <f aca="false">MAX(0,L$1*C16-K16)</f>
         <v>12</v>
       </c>
@@ -1128,24 +1204,24 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J17" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="J17" s="5" t="n">
         <f aca="false">MAX(0,L$1*C17-K17)</f>
         <v>6</v>
       </c>
@@ -1155,24 +1231,24 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="J18" s="5" t="n">
         <f aca="false">MAX(0,L$1*C18-K18)</f>
         <v>12</v>
       </c>
@@ -1182,24 +1258,24 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="J19" s="5" t="n">
         <f aca="false">MAX(0,L$1*C19-K19)</f>
         <v>6</v>
       </c>
@@ -1209,24 +1285,24 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J20" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="J20" s="5" t="n">
         <f aca="false">MAX(0,L$1*C20-K20)</f>
         <v>6</v>
       </c>
@@ -1236,27 +1312,27 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J21" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="J21" s="5" t="n">
         <f aca="false">MAX(0,L$1*C21-K21)</f>
         <v>3</v>
       </c>
@@ -1266,27 +1342,27 @@
         <v>1</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J22" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="J22" s="5" t="n">
         <f aca="false">MAX(0,L$1*C22-K22)</f>
         <v>3</v>
       </c>
@@ -1296,27 +1372,27 @@
         <v>1</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="J23" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="J23" s="5" t="n">
         <f aca="false">MAX(0,L$1*C23-K23)</f>
         <v>3</v>
       </c>
@@ -1326,30 +1402,30 @@
         <v>1</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>118</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J24" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="J24" s="5" t="n">
         <f aca="false">MAX(0,L$1*C24-K24)</f>
         <v>3</v>
       </c>
@@ -1359,27 +1435,27 @@
         <v>1</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="J25" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="J25" s="5" t="n">
         <f aca="false">MAX(0,L$1*C25-K25)</f>
         <v>3</v>
       </c>
@@ -1389,24 +1465,24 @@
         <v>1</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J26" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="J26" s="5" t="n">
         <f aca="false">MAX(0,L$1*C26-K26)</f>
         <v>3</v>
       </c>
@@ -1416,27 +1492,27 @@
         <v>1</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="J27" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="J27" s="5" t="n">
         <f aca="false">MAX(0,L$1*C27-K27)</f>
         <v>3</v>
       </c>
@@ -1446,27 +1522,27 @@
         <v>1</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="J28" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="J28" s="5" t="n">
         <f aca="false">MAX(0,L$1*C28-K28)</f>
         <v>3</v>
       </c>
@@ -1476,30 +1552,30 @@
         <v>1</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>147</v>
-      </c>
       <c r="H29" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="1" t="n">
+        <v>152</v>
+      </c>
+      <c r="J29" s="5" t="n">
         <f aca="false">MAX(0,L$1*C29-K29)</f>
         <v>3</v>
       </c>
@@ -1509,27 +1585,27 @@
         <v>1</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E30" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="F30" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>153</v>
-      </c>
       <c r="H30" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="J30" s="1" t="n">
+        <v>157</v>
+      </c>
+      <c r="J30" s="5" t="n">
         <f aca="false">MAX(0,L$1*C30-K30)</f>
         <v>3</v>
       </c>
@@ -1539,27 +1615,27 @@
         <v>1</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>158</v>
-      </c>
       <c r="H31" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="J31" s="1" t="n">
+        <v>161</v>
+      </c>
+      <c r="J31" s="5" t="n">
         <f aca="false">MAX(0,L$1*C31-K31)</f>
         <v>12</v>
       </c>

</xml_diff>